<commit_message>
VI Arrest Data 2008
</commit_message>
<xml_diff>
--- a/2008/vi-arrest-data-drug-arrests-2008.xlsx
+++ b/2008/vi-arrest-data-drug-arrests-2008.xlsx
@@ -4,7 +4,6 @@
   <workbookPr/>
   <sheets>
     <sheet sheetId="1" name="drug-arrests-by-age-and-type-of" state="visible" r:id="rId3"/>
-    <sheet sheetId="2" name="monthly-time-chart" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -109,56 +108,11 @@
   <si>
     <t>Total</t>
   </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>January</t>
-  </si>
-  <si>
-    <t>February</t>
-  </si>
-  <si>
-    <t>March</t>
-  </si>
-  <si>
-    <t>April</t>
-  </si>
-  <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>June</t>
-  </si>
-  <si>
-    <t>July</t>
-  </si>
-  <si>
-    <t>August</t>
-  </si>
-  <si>
-    <t>September</t>
-  </si>
-  <si>
-    <t>October</t>
-  </si>
-  <si>
-    <t>November</t>
-  </si>
-  <si>
-    <t>December</t>
-  </si>
-  <si>
-    <t>Number of Drug Arrests</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,###"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -192,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment/>
@@ -209,9 +163,6 @@
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="164" borderId="1" applyFont="1" fontId="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -222,10 +173,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -1678,101 +1625,4 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" customWidth="1" max="1" width="31.43"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c t="s" s="4" r="A1">
-        <v>32</v>
-      </c>
-      <c t="s" s="4" r="B1">
-        <v>33</v>
-      </c>
-      <c t="s" s="4" r="C1">
-        <v>34</v>
-      </c>
-      <c t="s" s="4" r="D1">
-        <v>35</v>
-      </c>
-      <c t="s" s="4" r="E1">
-        <v>36</v>
-      </c>
-      <c t="s" s="4" r="F1">
-        <v>37</v>
-      </c>
-      <c t="s" s="4" r="G1">
-        <v>38</v>
-      </c>
-      <c t="s" s="4" r="H1">
-        <v>39</v>
-      </c>
-      <c t="s" s="4" r="I1">
-        <v>40</v>
-      </c>
-      <c t="s" s="4" r="J1">
-        <v>41</v>
-      </c>
-      <c t="s" s="4" r="K1">
-        <v>42</v>
-      </c>
-      <c t="s" s="4" r="L1">
-        <v>43</v>
-      </c>
-      <c t="s" s="4" r="M1">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2">
-      <c t="s" s="4" r="A2">
-        <v>45</v>
-      </c>
-      <c s="6" r="B2">
-        <v>2821.0</v>
-      </c>
-      <c s="6" r="C2">
-        <v>2984.0</v>
-      </c>
-      <c s="6" r="D2">
-        <v>3444.0</v>
-      </c>
-      <c s="6" r="E2">
-        <v>3004.0</v>
-      </c>
-      <c s="6" r="F2">
-        <v>2989.0</v>
-      </c>
-      <c s="6" r="G2">
-        <v>2854.0</v>
-      </c>
-      <c s="6" r="H2">
-        <v>3001.0</v>
-      </c>
-      <c s="6" r="I2">
-        <v>2842.0</v>
-      </c>
-      <c s="6" r="J2">
-        <v>2581.0</v>
-      </c>
-      <c s="6" r="K2">
-        <v>2287.0</v>
-      </c>
-      <c s="6" r="L2">
-        <v>2174.0</v>
-      </c>
-      <c s="6" r="M2">
-        <v>2236.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>